<commit_message>
Moved economy-tables to new path for ontology schemes
</commit_message>
<xml_diff>
--- a/sources/fact_extraction_viewpoint/economy-table35.xlsx
+++ b/sources/fact_extraction_viewpoint/economy-table35.xlsx
@@ -52,7 +52,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -236,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -258,11 +258,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="38">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1576,7 +1584,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="ROW LABLE">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="ROW LABLE">
   <location ref="A3:B88" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -1908,7 +1916,29 @@
   <dataFields count="1">
     <dataField name="Sum of Amount" fld="2" baseField="6" baseItem="4" numFmtId="3"/>
   </dataFields>
-  <formats count="37">
+  <formats count="38">
+    <format dxfId="37">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="5">
+          <reference field="0" count="2">
+            <x v="0"/>
+            <x v="4"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="36">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
@@ -1926,34 +1956,12 @@
             <x v="0"/>
           </reference>
           <reference field="6" count="1" selected="0">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="35">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="5">
-          <reference field="0" count="2">
-            <x v="0"/>
-            <x v="4"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="2">
@@ -1975,7 +1983,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="34">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="2">
@@ -1997,13 +2005,13 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="33">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
     <format dxfId="32">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
     <format dxfId="31">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
-    </format>
-    <format dxfId="30">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="2">
@@ -2025,6 +2033,29 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="30">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="5">
+          <reference field="0" count="3">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="29">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
@@ -2043,35 +2074,12 @@
             <x v="1"/>
           </reference>
           <reference field="6" count="1" selected="0">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="28">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="5">
-          <reference field="0" count="3">
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="3">
@@ -2094,7 +2102,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="27">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="3">
@@ -2117,7 +2125,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="26">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="3">
@@ -2140,6 +2148,28 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="25">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="5">
+          <reference field="0" count="2">
+            <x v="0"/>
+            <x v="4"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="24">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
@@ -2157,34 +2187,12 @@
             <x v="0"/>
           </reference>
           <reference field="6" count="1" selected="0">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="23">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="5">
-          <reference field="0" count="2">
-            <x v="0"/>
-            <x v="4"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="2">
@@ -2206,7 +2214,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="2">
@@ -2228,7 +2236,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="2">
@@ -2250,6 +2258,29 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="20">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="5">
+          <reference field="0" count="3">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+          </reference>
+          <reference field="3" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="6" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
     <format dxfId="19">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
@@ -2268,35 +2299,12 @@
             <x v="1"/>
           </reference>
           <reference field="6" count="1" selected="0">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </format>
     <format dxfId="18">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="5">
-          <reference field="0" count="3">
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-          </reference>
-          <reference field="3" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="6" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="3">
@@ -2319,7 +2327,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="16">
+    <format dxfId="17">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="3">
@@ -2342,7 +2350,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="15">
+    <format dxfId="16">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="5">
           <reference field="0" count="3">
@@ -2365,19 +2373,34 @@
         </references>
       </pivotArea>
     </format>
+    <format dxfId="15">
+      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
     <format dxfId="14">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
     <format dxfId="13">
-      <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="4" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="12">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="3">
+          <reference field="3" count="1">
+            <x v="0"/>
+          </reference>
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
             <x v="0"/>
           </reference>
         </references>
@@ -2387,7 +2410,7 @@
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
           <reference field="4" count="1" selected="0">
             <x v="0"/>
@@ -2399,27 +2422,27 @@
       </pivotArea>
     </format>
     <format dxfId="10">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1">
-            <x v="1"/>
+            <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
             <x v="0"/>
           </reference>
           <reference field="5" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="9">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="4" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1">
             <x v="1"/>
           </reference>
         </references>
@@ -2429,7 +2452,7 @@
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
           <reference field="4" count="1" selected="0">
             <x v="0"/>
@@ -2441,27 +2464,27 @@
       </pivotArea>
     </format>
     <format dxfId="7">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1">
-            <x v="1"/>
+            <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
           <reference field="5" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="6">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="5" count="1">
             <x v="0"/>
           </reference>
         </references>
@@ -2471,7 +2494,7 @@
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
           <reference field="4" count="1" selected="0">
             <x v="1"/>
@@ -2483,27 +2506,27 @@
       </pivotArea>
     </format>
     <format dxfId="4">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="5" count="1">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1">
-            <x v="1"/>
+            <x v="0"/>
           </reference>
           <reference field="4" count="1" selected="0">
             <x v="1"/>
           </reference>
           <reference field="5" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="3">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="2">
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="5" count="1">
             <x v="1"/>
           </reference>
         </references>
@@ -2513,7 +2536,7 @@
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="3">
           <reference field="3" count="1">
-            <x v="0"/>
+            <x v="1"/>
           </reference>
           <reference field="4" count="1" selected="0">
             <x v="1"/>
@@ -2525,22 +2548,10 @@
       </pivotArea>
     </format>
     <format dxfId="1">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="3">
-          <reference field="3" count="1">
-            <x v="1"/>
-          </reference>
-          <reference field="4" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
     <format dxfId="0">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
   <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
@@ -2842,8 +2853,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:B88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -3536,7 +3547,7 @@
       <c r="A88" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="9">
         <v>178912.5</v>
       </c>
     </row>

</xml_diff>